<commit_message>
started on the cleaning and preprocessing
</commit_message>
<xml_diff>
--- a/desired_data_structure.xlsx
+++ b/desired_data_structure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idahelenedencker/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idahelenedencker/Desktop/STANDBY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EB1086-EC67-3D4F-B4C7-FEB7BFB78D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1F7A92-3E88-3848-8F13-E18CB9CF4910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="500" windowWidth="18580" windowHeight="15660" xr2:uid="{35B45B0C-289D-B541-98D0-FF19E16A6D61}"/>
+    <workbookView xWindow="5720" yWindow="500" windowWidth="22780" windowHeight="15660" xr2:uid="{35B45B0C-289D-B541-98D0-FF19E16A6D61}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>authorName</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>https://www.facebook.com/photo/?fbid=643551224456012&amp;amp;set=a.215836090560863&amp;amp;__cft__[0]=AZXX3Fc6-</t>
+  </si>
+  <si>
+    <t>date_data_collection</t>
+  </si>
+  <si>
+    <t>0505</t>
+  </si>
+  <si>
+    <t>identification</t>
   </si>
 </sst>
 </file>
@@ -279,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 Tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -319,7 +328,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -425,7 +434,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -567,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -575,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB2B6628-6529-E142-B4ED-6819B6E50981}">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:V1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -601,9 +610,10 @@
     <col min="23" max="23" width="16.6640625" customWidth="1"/>
     <col min="25" max="25" width="25.5" customWidth="1"/>
     <col min="26" max="26" width="15.5" customWidth="1"/>
+    <col min="27" max="27" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:28">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -682,8 +692,14 @@
       <c r="Z1" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:28">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -762,8 +778,14 @@
       <c r="Z2" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="AA2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:28">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -828,8 +850,11 @@
       <c r="Z3" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:28">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -894,8 +919,11 @@
       <c r="Z4" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="AB4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:28">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -960,14 +988,17 @@
       <c r="Z5" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="18">
+    <row r="6" spans="1:28" ht="18">
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:28">
       <c r="K7" s="1"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:28">
       <c r="D10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
@@ -976,7 +1007,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:28">
       <c r="H12" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working more on preprocessing
</commit_message>
<xml_diff>
--- a/desired_data_structure.xlsx
+++ b/desired_data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idahelenedencker/Desktop/STANDBY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1F7A92-3E88-3848-8F13-E18CB9CF4910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38C3B64-BF94-794C-991F-D99D3A437CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="500" windowWidth="22780" windowHeight="15660" xr2:uid="{35B45B0C-289D-B541-98D0-FF19E16A6D61}"/>
+    <workbookView xWindow="2160" yWindow="500" windowWidth="22780" windowHeight="15660" xr2:uid="{35B45B0C-289D-B541-98D0-FF19E16A6D61}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>authorName</t>
   </si>
@@ -158,9 +158,6 @@
     <t>count_wow</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>offentlig</t>
   </si>
   <si>
@@ -192,6 +189,15 @@
   </si>
   <si>
     <t>identification</t>
+  </si>
+  <si>
+    <t>offentlig_privat</t>
+  </si>
+  <si>
+    <t>name_abbreviation</t>
+  </si>
+  <si>
+    <t>BeJe</t>
   </si>
 </sst>
 </file>
@@ -584,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB2B6628-6529-E142-B4ED-6819B6E50981}">
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -611,9 +617,10 @@
     <col min="25" max="25" width="25.5" customWidth="1"/>
     <col min="26" max="26" width="15.5" customWidth="1"/>
     <col min="27" max="27" width="23.83203125" customWidth="1"/>
+    <col min="29" max="29" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:29">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -624,22 +631,22 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>2</v>
@@ -693,13 +700,16 @@
         <v>23</v>
       </c>
       <c r="AA1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
+        <v>50</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -710,16 +720,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>
@@ -770,7 +780,7 @@
         <v>25</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>24</v>
@@ -779,13 +789,16 @@
         <v>28</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AB2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:28">
+      <c r="AC2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -853,8 +866,11 @@
       <c r="AB3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:28">
+      <c r="AC3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -922,8 +938,11 @@
       <c r="AB4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:28">
+      <c r="AC4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -991,14 +1010,33 @@
       <c r="AB5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="18">
+      <c r="AC5" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="18">
       <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:28">
+      <c r="AB6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="K7" s="1"/>
-    </row>
-    <row r="10" spans="1:28">
+      <c r="AB7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="AB8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="AB9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="D10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
@@ -1006,8 +1044,16 @@
       <c r="J10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-    </row>
-    <row r="12" spans="1:28">
+      <c r="AB10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="AB11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="H12" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new files and changes to existing files
</commit_message>
<xml_diff>
--- a/desired_data_structure.xlsx
+++ b/desired_data_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idahelenedencker/Desktop/STANDBY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C8C2E2-A111-3B45-BD44-B99A02754CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A5886B-9414-EE40-BBB1-997193839731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7540" yWindow="500" windowWidth="22780" windowHeight="15660" xr2:uid="{35B45B0C-289D-B541-98D0-FF19E16A6D61}"/>
+    <workbookView xWindow="6020" yWindow="500" windowWidth="22780" windowHeight="15660" xr2:uid="{35B45B0C-289D-B541-98D0-FF19E16A6D61}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>authorName</t>
   </si>
@@ -216,6 +216,15 @@
   </si>
   <si>
     <t>aarhus</t>
+  </si>
+  <si>
+    <t>compliance</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -287,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -303,9 +312,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -621,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB2B6628-6529-E142-B4ED-6819B6E50981}">
-  <dimension ref="A1:AE17"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,7 +660,7 @@
     <col min="29" max="29" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -683,73 +689,76 @@
         <v>39</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="L1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -778,16 +787,16 @@
         <v>40</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>27</v>
@@ -799,38 +808,38 @@
         <v>27</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="2">
-        <v>1</v>
-      </c>
-      <c r="W2" s="7">
+      <c r="W2" s="2">
+        <v>1</v>
+      </c>
+      <c r="X2" s="2">
         <v>3</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Y2" s="2">
         <v>10</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Z2" s="2">
         <v>8</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AA2" s="2">
         <v>2</v>
       </c>
-      <c r="AA2" s="2">
-        <v>0</v>
-      </c>
       <c r="AB2" s="2">
         <v>0</v>
       </c>
@@ -843,8 +852,11 @@
       <c r="AE2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -873,55 +885,55 @@
         <v>40</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="2">
         <v>12345</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V3" s="2">
-        <v>1</v>
-      </c>
-      <c r="W3" s="7">
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2">
         <v>3</v>
       </c>
-      <c r="X3" s="2">
-        <v>1</v>
-      </c>
       <c r="Y3" s="2">
         <v>1</v>
       </c>
       <c r="Z3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="2">
         <v>0</v>
@@ -938,8 +950,11 @@
       <c r="AE3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -968,50 +983,50 @@
         <v>40</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>87654</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>12345</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="T4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="2">
-        <v>1</v>
-      </c>
-      <c r="W4" s="7">
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="2">
         <v>3</v>
       </c>
-      <c r="X4" s="2">
-        <v>0</v>
-      </c>
       <c r="Y4" s="2">
         <v>0</v>
       </c>
@@ -1033,8 +1048,11 @@
       <c r="AE4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1063,58 +1081,58 @@
         <v>40</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>55555</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="T5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V5" s="2">
-        <v>1</v>
-      </c>
-      <c r="W5" s="7">
+      <c r="W5" s="2">
+        <v>1</v>
+      </c>
+      <c r="X5" s="2">
         <v>3</v>
       </c>
-      <c r="X5" s="2">
-        <v>1</v>
-      </c>
       <c r="Y5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5" s="2">
         <v>0</v>
@@ -1128,42 +1146,48 @@
       <c r="AE5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1181,10 +1205,10 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="7"/>
+      <c r="W12" s="2"/>
       <c r="X12" s="2"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1202,10 +1226,10 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-      <c r="W13" s="7"/>
+      <c r="W13" s="2"/>
       <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1223,7 +1247,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="7"/>
+      <c r="W14" s="2"/>
       <c r="X14" s="2"/>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.2">

</xml_diff>